<commit_message>
Prace nad OMS parserem
</commit_message>
<xml_diff>
--- a/docs/SonicoBrudnopis.xlsx
+++ b/docs/SonicoBrudnopis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekty\Sonico\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\Python\LoRaFrameParser\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C072478A-14C2-482F-A58E-16CD5DDC5B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E3884D-8FA3-4446-9FEC-AF768D7FE15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46704" yWindow="972" windowWidth="8628" windowHeight="10740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1290" yWindow="1635" windowWidth="8490" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>uAh</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>External temperature</t>
+  </si>
+  <si>
+    <t>TU CHYBA JEST BŁĄD</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -434,13 +437,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>5/60</f>
         <v>8.3333333333333329E-2</v>
@@ -461,7 +464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -477,7 +480,7 @@
         <v>3.2538486568066589</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.59195</v>
       </c>
@@ -485,7 +488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6*3600</f>
         <v>5731.0199999999995</v>
@@ -494,7 +497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7/1000</f>
         <v>5.7310199999999991</v>
@@ -503,17 +506,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -521,7 +524,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -529,7 +532,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -537,7 +540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -545,7 +548,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -553,15 +556,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -569,7 +575,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -577,7 +583,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>

</xml_diff>

<commit_message>
LittleEndian added + table instead of text
</commit_message>
<xml_diff>
--- a/docs/SonicoBrudnopis.xlsx
+++ b/docs/SonicoBrudnopis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IT\Python\LoRaFrameParser\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekty\Sonico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E3884D-8FA3-4446-9FEC-AF768D7FE15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E9B996-D26F-49C7-92AA-B65BC4A7A973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1290" yWindow="1635" windowWidth="8490" windowHeight="11880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="44">
   <si>
     <t>uAh</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Ramka OMS (FrameCounter 38)</t>
   </si>
   <si>
-    <t>0411A15A993B441100000000426C244C02FD74000004FD17032C0004913C5E6F0100033933F9310259114202657D0B</t>
-  </si>
-  <si>
     <t xml:space="preserve">04 11 A15A993B </t>
   </si>
   <si>
@@ -65,9 +62,6 @@
     <t>02 FD 74 0000</t>
   </si>
   <si>
-    <t>04 FD 17 032C00</t>
-  </si>
-  <si>
     <t>04 91 3C 5E6F0100</t>
   </si>
   <si>
@@ -107,7 +101,70 @@
     <t>External temperature</t>
   </si>
   <si>
-    <t>TU CHYBA JEST BŁĄD</t>
+    <t>000001000001000110100001010110101001100100111011</t>
+  </si>
+  <si>
+    <t>010001000001000100000000000000000000000000000000</t>
+  </si>
+  <si>
+    <t>01000010011011000010010001001100</t>
+  </si>
+  <si>
+    <t>0000001011111101011101000000000000000000</t>
+  </si>
+  <si>
+    <t>000001001111110100010111000000110010110000000000</t>
+  </si>
+  <si>
+    <t>00000100100100010011110001011110011011110000000100000000</t>
+  </si>
+  <si>
+    <t>0000001100111001001100111111100100110001</t>
+  </si>
+  <si>
+    <t>00000010010110010001000101000010</t>
+  </si>
+  <si>
+    <t>00000010011001010111110100001011</t>
+  </si>
+  <si>
+    <t>00000100000100011010000101011010100110010011101101000100000100010000000000000000000000000000000001000010011011000010010001001100000000101111110101110100000000000000000000000100111111010001011100000011001011000000000000000100100100010011110001011110011011110000000100000000</t>
+  </si>
+  <si>
+    <t>01011110 01101111 00000001 0000 0000</t>
+  </si>
+  <si>
+    <t>00111100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10010001 </t>
+  </si>
+  <si>
+    <t>00000100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1111101 </t>
+  </si>
+  <si>
+    <t>00010111</t>
+  </si>
+  <si>
+    <t>03 FD 17 032C00</t>
+  </si>
+  <si>
+    <t>0411A15A993B441100000000426C244C02FD74000003FD17032C0004913C5E6F0100033933F9310259114202657D0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04 11 3EB0983B </t>
+  </si>
+  <si>
+    <t>44 11 00000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02 FD 74 0000 </t>
+  </si>
+  <si>
+    <t>04FD17032C0004913CC2190200033933F9310259114202651B0C</t>
   </si>
 </sst>
 </file>
@@ -152,12 +209,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -435,15 +493,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:T30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>5/60</f>
         <v>8.3333333333333329E-2</v>
@@ -464,7 +525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -480,7 +541,7 @@
         <v>3.2538486568066589</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.59195</v>
       </c>
@@ -488,7 +549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6*3600</f>
         <v>5731.0199999999995</v>
@@ -497,7 +558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <f>A7/1000</f>
         <v>5.7310199999999991</v>
@@ -506,89 +567,162 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="G17" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>7</v>
       </c>
-      <c r="C16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" t="s">
-        <v>23</v>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>